<commit_message>
Columns Name has been standard
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponsingh.arumugaraj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydocs.msc.com/personal/jegadeesan_rameshbabu_msc_com/Documents/Technix24/Safe-Seas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A35CC2-021E-424D-BA9E-2FDCC344F9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{22A35CC2-021E-424D-BA9E-2FDCC344F9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F4FE17E-5124-4507-86CD-B9094BD1FB42}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E1FAAC5-D8CC-44DC-8B07-4CD65077567D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4E1FAAC5-D8CC-44DC-8B07-4CD65077567D}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -37,48 +37,155 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>incident_id</t>
-  </si>
-  <si>
-    <t>route_id</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>risk_score</t>
-  </si>
-  <si>
-    <t>load_port</t>
-  </si>
-  <si>
-    <t>discharge_port</t>
-  </si>
-  <si>
-    <t>coordinates</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Covai</t>
-  </si>
-  <si>
-    <t>Ehc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cbhdbc</t>
-  </si>
-  <si>
-    <t>dfvdfv</t>
-  </si>
-  <si>
-    <t>vdfvdfv</t>
-  </si>
-  <si>
-    <t>[51.5, -0.1], [40.7, -74.0], [76.7, -32.0]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[31.2304, 121.4737] ,
+[35.1796 , 129.0756],
+[22.3193 , 114.1694],
+[1.3521 , 103.8198] ,
+[6.9271 , 79.8612 ] ,
+[17.0151 , 54.0924] ,
+[21.4858 , 39.1925] ,
+[31.2653 , 32.3019] ,
+[37.9420 , 23.6462] ,
+[39.4699 , 0.3763 ] ,
+[51.9225 , 4.4791 ] </t>
+  </si>
+  <si>
+    <t>Shanghai
+,Busan
+,Hong Kong
+,Singapore
+,Colombo
+,Salalah
+,Jeddah
+,Port Said
+,Piraeus
+,Valencia
+,Rotterdam</t>
+  </si>
+  <si>
+    <t>Issues with cargo exceeding weight limits.</t>
+  </si>
+  <si>
+    <t>Miscommunication between ship, port, and logistics providers.</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Health Emergencies</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medical issues among crew affecting operations.</t>
+  </si>
+  <si>
+    <t>Fuel Costs</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Fluctuations in fuel prices affecting operating costs.</t>
+  </si>
+  <si>
+    <t>Storage Limitations</t>
+  </si>
+  <si>
+    <t>Limited space for storing goods at ports.</t>
+  </si>
+  <si>
+    <t>Overweight Cargo</t>
+  </si>
+  <si>
+    <t>Port Congestion</t>
+  </si>
+  <si>
+    <t>Delays caused by too many ships at a port.</t>
+  </si>
+  <si>
+    <t>Shipping Lane Crowding</t>
+  </si>
+  <si>
+    <t>High traffic in key shipping lanes causing delays.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Communication Breakdown</t>
+  </si>
+  <si>
+    <t>Financial Instability</t>
+  </si>
+  <si>
+    <t>Economic downturns affecting shipping demand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shanghai </t>
+  </si>
+  <si>
+    <t>Route_Id</t>
+  </si>
+  <si>
+    <t>Origin_Port</t>
+  </si>
+  <si>
+    <t>Destination_Port</t>
+  </si>
+  <si>
+    <t>Orgin_Port_Country</t>
+  </si>
+  <si>
+    <t>Destination_Port_Country</t>
+  </si>
+  <si>
+    <t>No_Of_Stops</t>
+  </si>
+  <si>
+    <t>Stops_Names</t>
+  </si>
+  <si>
+    <t>Stop_Points</t>
+  </si>
+  <si>
+    <t>Average_Transit_Days</t>
+  </si>
+  <si>
+    <t>Travel_Direction</t>
+  </si>
+  <si>
+    <t>Vessel_Type</t>
+  </si>
+  <si>
+    <t>No_Of_Travels</t>
+  </si>
+  <si>
+    <t>Total_Incidents_Count</t>
+  </si>
+  <si>
+    <t>Risk_Score</t>
+  </si>
+  <si>
+    <t>Incident_Id</t>
+  </si>
+  <si>
+    <t>Incident_Type</t>
+  </si>
+  <si>
+    <t>Incident_Date</t>
   </si>
 </sst>
 </file>
@@ -114,8 +221,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,57 +558,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8AEA-CDC4-44D4-AFAF-47C328DE7469}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="103" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="199.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="H2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -513,33 +653,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F311D8-4566-440E-8FDA-465B73DA53F1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -547,13 +696,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45070.581944444442</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -561,11 +716,198 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>45</v>
-      </c>
+      <c r="E3" s="1">
+        <v>45194.581944444442</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45055.581944444442</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44801.581944444442</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44994.581944444442</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44915.581944444442</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44791.581944444442</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45141.581944444442</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44773.581944444442</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45191.581944444442</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>